<commit_message>
Support list diy class
</commit_message>
<xml_diff>
--- a/Loader/Loader/Data/ExcelFile/ActivityLevel.xlsx
+++ b/Loader/Loader/Data/ExcelFile/ActivityLevel.xlsx
@@ -33,37 +33,37 @@
     <t>VipPriceSale</t>
   </si>
   <si>
-    <t>(vActivityRightDesc</t>
+    <t>(VActivityRightDesc</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>等级</t>
+  </si>
+  <si>
+    <t>当前等级的总经验</t>
+  </si>
+  <si>
+    <t>购买普通商城内物品时获得的折扣(1代表1%)</t>
+  </si>
+  <si>
+    <t>额外增加每次竞技结束时的金钱、经验奖励(1代表1%)</t>
+  </si>
+  <si>
+    <t>再次购买钻石会员折扣(1代表1%)</t>
+  </si>
+  <si>
+    <t>(我是注释</t>
   </si>
   <si>
     <t>a</t>
   </si>
   <si>
-    <t>)</t>
-  </si>
-  <si>
-    <t>等级</t>
-  </si>
-  <si>
-    <t>当前等级的总经验</t>
-  </si>
-  <si>
-    <t>购买普通商城内物品时获得的折扣(1代表1%)</t>
-  </si>
-  <si>
-    <t>额外增加每次竞技结束时的金钱、经验奖励(1代表1%)</t>
-  </si>
-  <si>
-    <t>再次购买钻石会员折扣(1代表1%)</t>
-  </si>
-  <si>
-    <t>(我是注释</t>
-  </si>
-  <si>
     <t>int</t>
-  </si>
-  <si>
-    <t>(TestStruct</t>
   </si>
   <si>
     <t>(</t>
@@ -74,10 +74,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -95,8 +95,107 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -125,9 +224,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -135,114 +233,16 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -261,25 +261,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -291,151 +435,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -488,30 +488,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -523,6 +499,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -577,6 +562,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -593,10 +593,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -605,136 +605,136 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
@@ -1133,7 +1133,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6"/>
@@ -1195,13 +1195,13 @@
         <v>13</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="K2" t="s">
         <v>7</v>
@@ -1209,25 +1209,25 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="K3" t="s">
         <v>7</v>

</xml_diff>